<commit_message>
Added Steam Pipe Sound
</commit_message>
<xml_diff>
--- a/Planung/Ablauf.xlsx
+++ b/Planung/Ablauf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah Wiederhold\Desktop\Design_Sound\Planung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CA7E62-4D30-462C-AECB-8882F272B6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CD93A9-E7D1-48C3-AE62-2DFAB9F8286A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
   <si>
     <t>Details</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>fertig zum Einfügen in Game</t>
   </si>
 </sst>
 </file>
@@ -269,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -294,11 +297,98 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF02BE76"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5B5B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF02BE76"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5B5B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF02BE76"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF02BE76"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -631,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,7 +928,7 @@
         <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3">
@@ -893,8 +983,8 @@
         <v>28</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="3" t="s">
-        <v>25</v>
+      <c r="D13" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>29</v>
@@ -1028,7 +1118,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>5</v>
@@ -1340,7 +1430,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H5:L24">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1352,27 +1442,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D17 D19:D22">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="anzupassen">
-      <formula>NOT(ISERROR(SEARCH("anzupassen",D7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="zu bearbeiten">
+    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="zu bearbeiten">
       <formula>NOT(ISERROR(SEARCH("zu bearbeiten",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="zu erstellen">
+    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="zu erstellen">
       <formula>NOT(ISERROR(SEARCH("zu erstellen",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="anzupassen an Game">
-      <formula>NOT(ISERROR(SEARCH("anzupassen an Game",D18)))</formula>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="zu erstellen">
+      <formula>NOT(ISERROR(SEARCH("zu erstellen",D1)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="zu erstellen">
       <formula>NOT(ISERROR(SEARCH("zu erstellen",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="zu erstellen">
-      <formula>NOT(ISERROR(SEARCH("zu erstellen",D1)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="fertig zum Einfügen in Game">
+      <formula>NOT(ISERROR(SEARCH("fertig zum Einfügen in Game",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ablauf geändert und Flugzeug Hangar Sound Projekt angelegt
</commit_message>
<xml_diff>
--- a/Planung/Ablauf.xlsx
+++ b/Planung/Ablauf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah Wiederhold\Desktop\Design_Sound\Planung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CD93A9-E7D1-48C3-AE62-2DFAB9F8286A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E000412A-A6AB-47DE-BF90-D5065B8F1503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,7 +304,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -337,97 +337,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF02BE76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5B5B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF02BE76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF02BE76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5B5B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF02BE76"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF37A76F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -721,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,7 +837,7 @@
         <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3">
@@ -956,7 +865,7 @@
         <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Drache Sound + Weltraumtheme added
</commit_message>
<xml_diff>
--- a/Planung/Ablauf.xlsx
+++ b/Planung/Ablauf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah Wiederhold\Desktop\Design_Sound\Planung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E000412A-A6AB-47DE-BF90-D5065B8F1503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDCB6A3-BBEE-46DB-A476-EF3D312EA663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="47">
   <si>
     <t>Details</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>fertig zum Einfügen in Game</t>
+  </si>
+  <si>
+    <t>Weltraum Theme (Dark)</t>
+  </si>
+  <si>
+    <t>Loop-fähig</t>
   </si>
 </sst>
 </file>
@@ -630,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,16 +1170,28 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="3">
+        <v>10</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="I23" s="4"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="L23" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>

</xml_diff>

<commit_message>
Robot und Marsmännchen Sounds hinzugefügt
</commit_message>
<xml_diff>
--- a/Planung/Ablauf.xlsx
+++ b/Planung/Ablauf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah Wiederhold\Desktop\Design_Sound\Planung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDCB6A3-BBEE-46DB-A476-EF3D312EA663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03D4FA3-953C-4656-8FAA-56D4CF84BCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
   <si>
     <t>Details</t>
   </si>
@@ -132,21 +132,9 @@
     <t>Disturbance Noise</t>
   </si>
   <si>
-    <t>Character Sound Yippi</t>
-  </si>
-  <si>
     <t>bei Auswahl eines bestimmten Characters</t>
   </si>
   <si>
-    <t>Character Sound Here we go again</t>
-  </si>
-  <si>
-    <t>Character Sound Knurren</t>
-  </si>
-  <si>
-    <t>Character Sound Alien Geräusche</t>
-  </si>
-  <si>
     <t>Aufgaben nach Priorität markiertt:</t>
   </si>
   <si>
@@ -166,6 +154,36 @@
   </si>
   <si>
     <t>Loop-fähig</t>
+  </si>
+  <si>
+    <t>Character Sound Alien Oktopus</t>
+  </si>
+  <si>
+    <t>Character Sound Drache</t>
+  </si>
+  <si>
+    <t>Character Sound Roboter</t>
+  </si>
+  <si>
+    <t>Character Sound Marsmännchen</t>
+  </si>
+  <si>
+    <t>Character Sound Spaceman</t>
+  </si>
+  <si>
+    <t>Drachenlord in mein Audi Hook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Technik siegt" mit sehr viel spacigen Effekten </t>
+  </si>
+  <si>
+    <t>"Erdlinge müssen vernichtet werden" mit Verzerrung</t>
+  </si>
+  <si>
+    <t>"Für die Galaxys" mit heroischer Stimme</t>
+  </si>
+  <si>
+    <t>glibschiger Sound (Ork Geräusch pitchen mit Effekten)</t>
   </si>
 </sst>
 </file>
@@ -310,11 +328,11 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF02BE76"/>
+          <bgColor rgb="FFFF5B5B"/>
         </patternFill>
       </fill>
     </dxf>
@@ -328,7 +346,28 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF02BE76"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF5B5B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF02BE76"/>
         </patternFill>
       </fill>
     </dxf>
@@ -634,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:L46"/>
+  <dimension ref="B3:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,10 +695,10 @@
   <sheetData>
     <row r="3" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -811,7 +850,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>21</v>
@@ -868,10 +907,10 @@
         <v>26</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>27</v>
@@ -899,7 +938,7 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>29</v>
@@ -1033,7 +1072,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>5</v>
@@ -1059,23 +1098,25 @@
     </row>
     <row r="19" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="F19" s="3">
         <v>20</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>12</v>
@@ -1087,23 +1128,25 @@
     </row>
     <row r="20" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="F20" s="3">
         <v>20</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>12</v>
@@ -1115,23 +1158,25 @@
     </row>
     <row r="21" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="F21" s="3">
         <v>20</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>12</v>
@@ -1143,23 +1188,25 @@
     </row>
     <row r="22" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F22" s="3">
         <v>20</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>12</v>
@@ -1171,46 +1218,71 @@
     </row>
     <row r="23" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="3">
+        <v>20</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="3">
-        <v>10</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="5"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
+      <c r="H24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="2:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6"/>
@@ -1352,11 +1424,18 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F47" s="6"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H5:L24">
+  <conditionalFormatting sqref="H5:L18 H24:L25 I19:L23">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -1368,23 +1447,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D17 D19:D22">
-    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="zu bearbeiten">
+  <conditionalFormatting sqref="D7:D17 D19:D23">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="zu bearbeiten">
       <formula>NOT(ISERROR(SEARCH("zu bearbeiten",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="zu erstellen">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="zu erstellen">
       <formula>NOT(ISERROR(SEARCH("zu erstellen",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="zu erstellen">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="fertig zum Einfügen in Game">
+      <formula>NOT(ISERROR(SEARCH("fertig zum Einfügen in Game",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="zu erstellen">
       <formula>NOT(ISERROR(SEARCH("zu erstellen",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="zu erstellen">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="zu erstellen">
       <formula>NOT(ISERROR(SEARCH("zu erstellen",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="fertig zum Einfügen in Game">
-      <formula>NOT(ISERROR(SEARCH("fertig zum Einfügen in Game",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>